<commit_message>
Antwort 1-100 und neue Excel Datei
</commit_message>
<xml_diff>
--- a/files/Fragen.xlsx
+++ b/files/Fragen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lgsachsenheim-my.sharepoint.com/personal/golze_paul_elgs_schulportal_schulstiftung_info/Documents/IMP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{967E1FA5-083F-4F1F-80BF-E7B83A88412B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C7A3DB-E3BB-451D-A8FF-431184D5AC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{FEFB16A5-D4A0-4625-B94E-FC4230FEBFEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FEFB16A5-D4A0-4625-B94E-FC4230FEBFEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,9 @@
   <commentList>
     <comment ref="T93" authorId="0" shapeId="0" xr:uid="{FD4F012B-4165-4CA4-8719-6EF93C4E1C66}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     ok</t>
       </text>
     </comment>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="137">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>BPM</t>
-  </si>
-  <si>
-    <t>Wo warst du um die Uhrzeit?</t>
   </si>
   <si>
     <t>Hast du ein Alibi?</t>
@@ -282,9 +279,6 @@
     <t>Wie ging es dir um 17:45 Uhr?</t>
   </si>
   <si>
-    <t>Hast du Punkte in Flensburg, wenn ja wie viele?</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                    </t>
   </si>
   <si>
@@ -360,9 +354,6 @@
     <t>Hast du um 15:45 Uhr mit jemanedem Kontakt gehabt?</t>
   </si>
   <si>
-    <t>Warst du noch nie in München?</t>
-  </si>
-  <si>
     <t>Sind sie in Bayern geboren?</t>
   </si>
   <si>
@@ -387,9 +378,6 @@
     <t>Hast du dich um 19:50 Uhr mit jemandem getroffen?</t>
   </si>
   <si>
-    <t>Wo warst an dem Tag? Gibt es irgendwelche Zeugen dafür?</t>
-  </si>
-  <si>
     <t>Würdest du lieber eine junge oder ältere Person töten?</t>
   </si>
   <si>
@@ -399,7 +387,100 @@
     <t>Bist du vorbestraft?</t>
   </si>
   <si>
-    <t>Was genau hast du am 18. August um 15:45 Uhr gemacht?</t>
+    <t>Antwort</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>6:30 Uhr</t>
+  </si>
+  <si>
+    <t>Arbeiten</t>
+  </si>
+  <si>
+    <t>Brot mit Käse</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>8 Stunden</t>
+  </si>
+  <si>
+    <t>Ich habe das nicht gemacht</t>
+  </si>
+  <si>
+    <t>Stuttgart</t>
+  </si>
+  <si>
+    <t>Deutsch</t>
+  </si>
+  <si>
+    <t>Schlecht</t>
+  </si>
+  <si>
+    <t>B, AM und L</t>
+  </si>
+  <si>
+    <t>Wo warst du um 9:00 Uhr?</t>
+  </si>
+  <si>
+    <t>Auf dem Weg zum Arbeiten</t>
+  </si>
+  <si>
+    <t>Jeans und T-Shirt</t>
+  </si>
+  <si>
+    <t>lebenslang im Gefängnis</t>
+  </si>
+  <si>
+    <t>7:00 Uhr</t>
+  </si>
+  <si>
+    <t>bewölkt</t>
+  </si>
+  <si>
+    <t>Ich war zuhause aber ohne Freundin</t>
+  </si>
+  <si>
+    <t>Von der Arbeit</t>
+  </si>
+  <si>
+    <t>gut</t>
+  </si>
+  <si>
+    <t>Wie viele Punkte in Flensburg hast du?</t>
+  </si>
+  <si>
+    <t>schwarz</t>
+  </si>
+  <si>
+    <t>Abendbrot gegessen</t>
+  </si>
+  <si>
+    <t>blau</t>
+  </si>
+  <si>
+    <t>regnerisch</t>
+  </si>
+  <si>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>zuhause</t>
+  </si>
+  <si>
+    <t>Deuscht</t>
+  </si>
+  <si>
+    <t>Ich habe keinen</t>
+  </si>
+  <si>
+    <t>Ältere Person</t>
+  </si>
+  <si>
+    <t>Was genau hast du um 15:45 Uhr gemacht?</t>
   </si>
 </sst>
 </file>
@@ -409,7 +490,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$₼-42C]\ * #,##0.00_-;\-[$₼-42C]\ * #,##0.00_-;_-[$₼-42C]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -669,7 +750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -821,6 +902,9 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -846,7 +930,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1152,16 +1236,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FE7B2B-B244-4DB1-96E1-1BBBEAD0F830}">
   <dimension ref="E1:T121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6:T6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="61" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.5703125" bestFit="1" customWidth="1"/>
@@ -1169,7 +1254,7 @@
     <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:20">
+    <row r="1" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E1" s="8"/>
       <c r="G1" t="s">
         <v>0</v>
@@ -1178,10 +1263,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="5:20">
+    <row r="4" spans="5:20" x14ac:dyDescent="0.25">
       <c r="I4" s="8"/>
     </row>
-    <row r="6" spans="5:20" ht="26.25">
+    <row r="6" spans="5:20" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="J6" s="36" t="s">
+        <v>105</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="36" t="s">
         <v>1</v>
@@ -1209,12 +1297,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="5:20">
+    <row r="7" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>108</v>
+      </c>
       <c r="K7" s="47">
         <v>1</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="M7" s="13" t="str">
         <f>I9</f>
@@ -1230,18 +1321,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="5:20">
+    <row r="8" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>106</v>
+      </c>
       <c r="K8" s="47">
         <v>2</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N8" s="55">
         <v>35.700000000000003</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2">
@@ -1251,18 +1345,21 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="5:20">
+    <row r="9" spans="5:20" x14ac:dyDescent="0.25">
       <c r="H9" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>13</v>
+      <c r="J9" t="s">
+        <v>106</v>
       </c>
       <c r="K9" s="47">
         <v>3</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1275,18 +1372,21 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="5:20">
+    <row r="10" spans="5:20" x14ac:dyDescent="0.25">
       <c r="H10" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="14" t="s">
-        <v>16</v>
+      <c r="J10" t="s">
+        <v>107</v>
       </c>
       <c r="K10" s="47">
         <v>4</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" s="13" t="str">
         <f>I9</f>
@@ -1302,18 +1402,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="5:20">
+    <row r="11" spans="5:20" x14ac:dyDescent="0.25">
       <c r="H11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>19</v>
       </c>
       <c r="K11" s="47">
         <v>5</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M11" s="2">
         <v>52</v>
@@ -1328,18 +1428,21 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="5:20">
+    <row r="12" spans="5:20" x14ac:dyDescent="0.25">
       <c r="H12" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>22</v>
+      <c r="J12" t="s">
+        <v>109</v>
       </c>
       <c r="K12" s="47">
         <v>6</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M12" s="13" t="str">
         <f>I9</f>
@@ -1355,18 +1458,21 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="5:20">
+    <row r="13" spans="5:20" x14ac:dyDescent="0.25">
       <c r="H13" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="17" t="s">
-        <v>25</v>
+      <c r="J13" t="s">
+        <v>110</v>
       </c>
       <c r="K13" s="47">
         <v>7</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M13" s="16" t="str">
         <f>I12</f>
@@ -1376,24 +1482,27 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R13" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="5:20">
+    <row r="14" spans="5:20" x14ac:dyDescent="0.25">
       <c r="H14" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="18" t="s">
-        <v>28</v>
+      <c r="J14" t="s">
+        <v>111</v>
       </c>
       <c r="K14" s="47">
         <v>8</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M14" s="22" t="str">
         <f>I16</f>
@@ -1409,25 +1518,28 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="5:20">
+    <row r="15" spans="5:20" x14ac:dyDescent="0.25">
       <c r="H15" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="19" t="s">
-        <v>31</v>
+      <c r="J15" t="s">
+        <v>112</v>
       </c>
       <c r="K15" s="47">
         <v>9</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2">
         <v>25</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2">
@@ -1437,18 +1549,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="5:20">
+    <row r="16" spans="5:20" x14ac:dyDescent="0.25">
       <c r="H16" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>34</v>
+      <c r="J16" t="s">
+        <v>110</v>
       </c>
       <c r="K16" s="47">
         <v>10</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M16" s="13" t="str">
         <f>I9</f>
@@ -1464,18 +1579,21 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="8:18">
+    <row r="17" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H17" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="31" t="s">
-        <v>37</v>
+      <c r="J17" t="s">
+        <v>110</v>
       </c>
       <c r="K17" s="47">
         <v>11</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M17" s="17" t="str">
         <f>I13</f>
@@ -1485,7 +1603,7 @@
         <v>64</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2">
@@ -1495,18 +1613,21 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="8:18">
+    <row r="18" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H18" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="42" t="s">
-        <v>41</v>
+      <c r="J18" t="s">
+        <v>106</v>
       </c>
       <c r="K18" s="47">
         <v>12</v>
       </c>
       <c r="L18" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M18" s="32" t="str">
         <f>I18</f>
@@ -1516,7 +1637,7 @@
         <v>94</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="2">
@@ -1526,18 +1647,21 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="8:18">
+    <row r="19" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H19" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="43" t="s">
-        <v>44</v>
+      <c r="J19" t="s">
+        <v>113</v>
       </c>
       <c r="K19" s="47">
         <v>13</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M19" s="18" t="str">
         <f>I14</f>
@@ -1553,18 +1677,21 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="8:18">
+    <row r="20" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H20" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="50" t="s">
-        <v>47</v>
+      <c r="J20" t="s">
+        <v>114</v>
       </c>
       <c r="K20" s="47">
         <v>14</v>
       </c>
       <c r="L20" s="54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M20" s="18" t="str">
         <f>I14</f>
@@ -1580,18 +1707,21 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="8:18">
+    <row r="21" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="I21" s="49" t="s">
-        <v>50</v>
+      <c r="J21" t="s">
+        <v>106</v>
       </c>
       <c r="K21" s="47">
         <v>15</v>
       </c>
       <c r="L21" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M21" s="22" t="str">
         <f>I16</f>
@@ -1607,12 +1737,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="8:18">
+    <row r="22" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>110</v>
+      </c>
       <c r="K22" s="47">
         <v>16</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M22" s="19" t="str">
         <f>I15</f>
@@ -1628,12 +1761,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="8:18">
+    <row r="23" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>110</v>
+      </c>
       <c r="K23" s="47">
         <v>17</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M23" s="19" t="str">
         <f>I15</f>
@@ -1649,15 +1785,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="8:18">
+    <row r="24" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>115</v>
+      </c>
       <c r="K24" s="47">
         <v>18</v>
       </c>
       <c r="L24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M24" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="M24" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1667,12 +1806,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="8:18">
+    <row r="25" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>116</v>
+      </c>
       <c r="K25" s="47">
         <v>19</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M25" s="39">
         <v>50.78</v>
@@ -1687,12 +1829,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="8:18">
+    <row r="26" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>110</v>
+      </c>
       <c r="K26" s="47">
         <v>20</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M26" s="16" t="str">
         <f>I12</f>
@@ -1708,12 +1853,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="8:18">
+    <row r="27" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>118</v>
+      </c>
       <c r="K27" s="47">
         <v>21</v>
       </c>
       <c r="L27" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M27" s="34" t="str">
         <f>I19</f>
@@ -1729,12 +1877,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="8:18">
+    <row r="28" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>119</v>
+      </c>
       <c r="K28" s="47">
         <v>22</v>
       </c>
       <c r="L28" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M28" s="51" t="str">
         <f>I21</f>
@@ -1748,12 +1899,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="8:18">
+    <row r="29" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>106</v>
+      </c>
       <c r="K29" s="2">
         <v>23</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1764,12 +1918,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="8:18">
+    <row r="30" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>120</v>
+      </c>
       <c r="K30" s="47">
         <v>24</v>
       </c>
       <c r="L30" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M30" s="24" t="str">
         <f>I17</f>
@@ -1785,22 +1942,25 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="8:18">
+    <row r="31" spans="8:18" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="J31" t="s">
+        <v>112</v>
       </c>
       <c r="K31" s="2">
         <v>25</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2">
         <v>9</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
@@ -1808,15 +1968,18 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="8:18">
+    <row r="32" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>121</v>
+      </c>
       <c r="K32" s="47">
         <v>26</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M32" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N32" s="2"/>
       <c r="P32" s="2"/>
@@ -1827,19 +1990,22 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="8:18">
+    <row r="33" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I33" s="53">
         <f>COUNTA(L7:L106)</f>
         <v>100</v>
       </c>
+      <c r="J33" t="s">
+        <v>122</v>
+      </c>
       <c r="K33" s="47">
         <v>27</v>
       </c>
       <c r="L33" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M33" s="52" t="str">
         <f>I20</f>
@@ -1853,19 +2019,22 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="8:18">
+    <row r="34" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I34" s="53">
         <f>COUNTA(R7:R106)</f>
         <v>100</v>
       </c>
+      <c r="J34" t="s">
+        <v>123</v>
+      </c>
       <c r="K34" s="47">
         <v>28</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M34" s="32" t="str">
         <f>I18</f>
@@ -1881,19 +2050,22 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="8:18">
+    <row r="35" spans="8:18" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I35" s="53">
         <f>COUNTA(O8:O107)</f>
         <v>10</v>
       </c>
+      <c r="J35" t="s">
+        <v>124</v>
+      </c>
       <c r="K35" s="47">
         <v>29</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M35" s="16" t="str">
         <f>I12</f>
@@ -1909,12 +2081,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="8:18">
+    <row r="36" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>125</v>
+      </c>
       <c r="K36" s="47">
         <v>30</v>
       </c>
       <c r="L36" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M36" s="34" t="str">
         <f>I19</f>
@@ -1928,19 +2103,22 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="8:18">
+    <row r="37" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J37" s="56">
+        <v>2</v>
+      </c>
       <c r="K37" s="47">
         <v>31</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="M37" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P37" s="2"/>
       <c r="Q37" s="2">
@@ -1950,12 +2128,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="8:18">
+    <row r="38" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>106</v>
+      </c>
       <c r="K38" s="47">
         <v>32</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M38" s="39">
         <v>45.68</v>
@@ -1970,12 +2151,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="8:18">
+    <row r="39" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>127</v>
+      </c>
       <c r="K39" s="47">
         <v>33</v>
       </c>
       <c r="L39" s="46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M39" s="51" t="str">
         <f>I21</f>
@@ -1989,12 +2173,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="8:18">
+    <row r="40" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>106</v>
+      </c>
       <c r="K40" s="47">
         <v>34</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M40" s="16" t="str">
         <f>I12</f>
@@ -2010,32 +2197,40 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="8:18">
+    <row r="41" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>106</v>
+      </c>
       <c r="K41" s="2">
         <v>35</v>
       </c>
-      <c r="L41" s="2" t="s">
-        <v>10</v>
+      <c r="L41" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="55">
         <v>2.7</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
+      <c r="Q41" s="2">
+        <v>3</v>
+      </c>
       <c r="R41" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="8:18">
+    <row r="42" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>128</v>
+      </c>
       <c r="K42" s="2">
         <v>36</v>
       </c>
       <c r="L42" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -2046,15 +2241,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="8:18">
+    <row r="43" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>106</v>
+      </c>
       <c r="K43" s="47">
         <v>37</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M43" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -2066,12 +2264,15 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="8:18">
+    <row r="44" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>119</v>
+      </c>
       <c r="K44" s="2">
         <v>38</v>
       </c>
       <c r="L44" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -2082,12 +2283,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="8:18">
+    <row r="45" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>106</v>
+      </c>
       <c r="K45" s="47">
         <v>39</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M45" s="17" t="str">
         <f>I13</f>
@@ -2103,12 +2307,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="8:18">
+    <row r="46" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>129</v>
+      </c>
       <c r="K46" s="47">
         <v>40</v>
       </c>
       <c r="L46" s="45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M46" s="51" t="str">
         <f>I21</f>
@@ -2122,12 +2329,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="8:18">
+    <row r="47" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>106</v>
+      </c>
       <c r="K47" s="28">
         <v>41</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M47" s="29"/>
       <c r="N47" s="2"/>
@@ -2138,12 +2348,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="8:18">
+    <row r="48" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>128</v>
+      </c>
       <c r="K48" s="48">
         <v>42</v>
       </c>
       <c r="L48" s="34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M48" s="34" t="str">
         <f>I19</f>
@@ -2159,12 +2372,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="11:18">
+    <row r="49" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>119</v>
+      </c>
       <c r="K49" s="2">
         <v>43</v>
       </c>
       <c r="L49" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -2175,12 +2391,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="11:18">
+    <row r="50" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K50" s="47">
         <v>44</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M50" s="13" t="str">
         <f>I9</f>
@@ -2196,12 +2412,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="11:18">
+    <row r="51" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>110</v>
+      </c>
       <c r="K51" s="2">
         <v>45</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M51" s="39">
         <v>32.68</v>
@@ -2214,12 +2433,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="11:18">
+    <row r="52" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>106</v>
+      </c>
       <c r="K52" s="2">
         <v>46</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -2230,15 +2452,18 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="11:18">
+    <row r="53" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>106</v>
+      </c>
       <c r="K53" s="47">
         <v>47</v>
       </c>
       <c r="L53" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M53" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -2250,12 +2475,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="11:18">
+    <row r="54" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>106</v>
+      </c>
       <c r="K54" s="2">
         <v>48</v>
       </c>
       <c r="L54" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -2266,12 +2494,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="11:18">
+    <row r="55" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K55" s="47">
         <v>49</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M55" s="32" t="str">
         <f>I18</f>
@@ -2287,12 +2515,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="11:18">
+    <row r="56" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>116</v>
+      </c>
       <c r="K56" s="2">
         <v>50</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M56" s="39">
         <v>19.78</v>
@@ -2307,12 +2538,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="11:18">
+    <row r="57" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>130</v>
+      </c>
       <c r="K57" s="47">
         <v>51</v>
       </c>
       <c r="L57" s="44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M57" s="52" t="str">
         <f>I18</f>
@@ -2326,12 +2560,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="11:18">
+    <row r="58" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K58" s="2">
         <v>52</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M58" s="2">
         <v>5</v>
@@ -2346,12 +2580,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="11:18">
+    <row r="59" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>131</v>
+      </c>
       <c r="K59" s="47">
         <v>53</v>
       </c>
       <c r="L59" s="46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M59" s="51" t="str">
         <f>I21</f>
@@ -2365,15 +2602,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="11:18">
+    <row r="60" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>106</v>
+      </c>
       <c r="K60" s="47">
         <v>54</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M60" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -2383,12 +2623,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="11:18">
+    <row r="61" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>132</v>
+      </c>
       <c r="K61" s="47">
         <v>55</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M61" s="3" t="str">
         <f>I9</f>
@@ -2404,12 +2647,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="11:18">
+    <row r="62" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>106</v>
+      </c>
       <c r="K62" s="47">
         <v>56</v>
       </c>
       <c r="L62" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M62" s="17" t="str">
         <f>I13</f>
@@ -2425,12 +2671,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="11:18">
+    <row r="63" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>110</v>
+      </c>
       <c r="K63" s="2">
         <v>57</v>
       </c>
       <c r="L63" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M63" s="27"/>
       <c r="N63" s="2"/>
@@ -2443,12 +2692,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="11:18">
+    <row r="64" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>110</v>
+      </c>
       <c r="K64" s="47">
         <v>58</v>
       </c>
       <c r="L64" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M64" s="16" t="str">
         <f>I12</f>
@@ -2462,12 +2714,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="11:18">
+    <row r="65" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>110</v>
+      </c>
       <c r="K65" s="47">
         <v>59</v>
       </c>
       <c r="L65" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M65" s="22" t="str">
         <f>I16</f>
@@ -2483,12 +2738,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="11:18">
+    <row r="66" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>127</v>
+      </c>
       <c r="K66" s="47">
         <v>60</v>
       </c>
       <c r="L66" s="46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M66" s="51" t="str">
         <f>I21</f>
@@ -2502,15 +2760,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="11:18">
+    <row r="67" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>106</v>
+      </c>
       <c r="K67" s="47">
         <v>61</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M67" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -2522,12 +2783,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="11:18">
+    <row r="68" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>106</v>
+      </c>
       <c r="K68" s="47">
         <v>62</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M68" s="13" t="str">
         <f>I9</f>
@@ -2543,12 +2807,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="11:18">
+    <row r="69" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>110</v>
+      </c>
       <c r="K69" s="47">
         <v>63</v>
       </c>
       <c r="L69" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M69" s="34" t="str">
         <f>I19</f>
@@ -2562,19 +2829,22 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="11:18">
+    <row r="70" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>110</v>
+      </c>
       <c r="K70" s="2">
         <v>64</v>
       </c>
-      <c r="L70" s="9" t="s">
-        <v>96</v>
+      <c r="L70" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="M70" s="17"/>
       <c r="N70" s="2">
         <v>11</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
@@ -2582,12 +2852,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="11:18">
+    <row r="71" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>106</v>
+      </c>
       <c r="K71" s="47">
         <v>65</v>
       </c>
       <c r="L71" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="M71" s="18" t="str">
         <f>I14</f>
@@ -2603,12 +2876,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="11:18">
+    <row r="72" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>122</v>
+      </c>
       <c r="K72" s="47">
         <v>66</v>
       </c>
       <c r="L72" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M72" s="52" t="str">
         <f>I20</f>
@@ -2622,12 +2898,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="11:18">
+    <row r="73" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>133</v>
+      </c>
       <c r="K73" s="47">
         <v>67</v>
       </c>
       <c r="L73" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M73" s="18" t="str">
         <f>I14</f>
@@ -2643,12 +2922,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="11:18">
+    <row r="74" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>110</v>
+      </c>
       <c r="K74" s="47">
         <v>68</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M74" s="39">
         <v>32.450000000000003</v>
@@ -2663,12 +2945,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="11:18">
+    <row r="75" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>106</v>
+      </c>
       <c r="K75" s="2">
         <v>69</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -2679,19 +2964,22 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="11:18">
+    <row r="76" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>106</v>
+      </c>
       <c r="K76" s="2">
         <v>70</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2">
         <v>2.35</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
@@ -2699,15 +2987,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="11:18">
+    <row r="77" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>106</v>
+      </c>
       <c r="K77" s="47">
         <v>71</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M77" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -2719,12 +3010,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="11:18">
+    <row r="78" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>123</v>
+      </c>
       <c r="K78" s="2">
         <v>72</v>
       </c>
       <c r="L78" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -2735,12 +3029,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="11:18">
+    <row r="79" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>106</v>
+      </c>
       <c r="K79" s="47">
         <v>73</v>
       </c>
       <c r="L79" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M79" s="19" t="str">
         <f>I15</f>
@@ -2756,12 +3053,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="11:18">
+    <row r="80" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>106</v>
+      </c>
       <c r="K80" s="2">
         <v>74</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
@@ -2772,12 +3072,15 @@
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="11:20">
+    <row r="81" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>128</v>
+      </c>
       <c r="K81" s="47">
         <v>75</v>
       </c>
       <c r="L81" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M81" s="34" t="str">
         <f>I19</f>
@@ -2793,12 +3096,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="82" spans="11:20">
+    <row r="82" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>110</v>
+      </c>
       <c r="K82" s="2">
         <v>76</v>
       </c>
       <c r="L82" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -2809,12 +3115,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="11:20">
+    <row r="83" spans="10:20" x14ac:dyDescent="0.25">
       <c r="K83" s="47">
         <v>77</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M83" s="13" t="str">
         <f>I9</f>
@@ -2830,12 +3136,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="11:20">
+    <row r="84" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J84" t="s">
+        <v>116</v>
+      </c>
       <c r="K84" s="47">
         <v>78</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M84" s="41">
         <v>19.5</v>
@@ -2850,12 +3159,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="11:20">
+    <row r="85" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J85" t="s">
+        <v>106</v>
+      </c>
       <c r="K85" s="2">
         <v>79</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -2866,12 +3178,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="11:20">
+    <row r="86" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>131</v>
+      </c>
       <c r="K86" s="47">
         <v>80</v>
       </c>
       <c r="L86" s="46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M86" s="51" t="str">
         <f>I21</f>
@@ -2885,12 +3200,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="11:20">
+    <row r="87" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>110</v>
+      </c>
       <c r="K87" s="47">
         <v>81</v>
       </c>
       <c r="L87" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M87" s="19" t="str">
         <f>I15</f>
@@ -2904,12 +3222,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="11:20">
+    <row r="88" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>134</v>
+      </c>
       <c r="K88" s="47">
         <v>82</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M88" s="20"/>
       <c r="N88" s="2"/>
@@ -2922,12 +3243,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="11:20">
+    <row r="89" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>130</v>
+      </c>
       <c r="K89" s="47">
         <v>83</v>
       </c>
       <c r="L89" s="44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M89" s="52" t="str">
         <f>I20</f>
@@ -2941,12 +3265,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="11:20">
+    <row r="90" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>106</v>
+      </c>
       <c r="K90" s="47">
         <v>84</v>
       </c>
       <c r="L90" s="23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M90" s="24" t="str">
         <f>I17</f>
@@ -2962,12 +3289,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="11:20">
+    <row r="91" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>106</v>
+      </c>
       <c r="K91" s="47">
         <v>85</v>
       </c>
       <c r="L91" s="33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M91" s="34" t="str">
         <f>I19</f>
@@ -2981,12 +3311,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="11:20">
+    <row r="92" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>128</v>
+      </c>
       <c r="K92" s="2">
         <v>86</v>
       </c>
       <c r="L92" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
@@ -2997,12 +3330,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="11:20">
+    <row r="93" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>110</v>
+      </c>
       <c r="K93" s="47">
         <v>87</v>
       </c>
-      <c r="L93" s="5" t="s">
-        <v>105</v>
+      <c r="L93" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="M93" s="32" t="str">
         <f>I18</f>
@@ -3018,12 +3354,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="11:20">
+    <row r="94" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J94" t="s">
+        <v>125</v>
+      </c>
       <c r="K94" s="47">
         <v>88</v>
       </c>
       <c r="L94" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M94" s="34" t="str">
         <f>I19</f>
@@ -3037,12 +3376,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="11:20">
+    <row r="95" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>119</v>
+      </c>
       <c r="K95" s="2">
         <v>89</v>
       </c>
       <c r="L95" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -3053,12 +3395,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="11:20">
+    <row r="96" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J96" t="s">
+        <v>135</v>
+      </c>
       <c r="K96" s="47">
         <v>90</v>
       </c>
       <c r="L96" s="23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="M96" s="24" t="str">
         <f>I17</f>
@@ -3074,12 +3419,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="11:18">
+    <row r="97" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>118</v>
+      </c>
       <c r="K97" s="2">
         <v>91</v>
       </c>
-      <c r="L97" s="5" t="s">
-        <v>66</v>
+      <c r="L97" s="33" t="s">
+        <v>57</v>
       </c>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
@@ -3090,12 +3438,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="11:18">
+    <row r="98" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>106</v>
+      </c>
       <c r="K98" s="47">
         <v>92</v>
       </c>
       <c r="L98" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M98" s="16" t="str">
         <f>I12</f>
@@ -3111,12 +3462,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="11:18">
+    <row r="99" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>106</v>
+      </c>
       <c r="K99" s="47">
         <v>93</v>
       </c>
       <c r="L99" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M99" s="24" t="str">
         <f>I17</f>
@@ -3132,19 +3486,22 @@
         <v>91</v>
       </c>
     </row>
-    <row r="100" spans="11:18">
+    <row r="100" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J100" t="s">
+        <v>106</v>
+      </c>
       <c r="K100" s="2">
         <v>94</v>
       </c>
       <c r="L100" s="32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="M100" s="2"/>
       <c r="N100" s="2">
         <v>12</v>
       </c>
       <c r="O100" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
@@ -3152,12 +3509,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="11:18">
+    <row r="101" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J101" t="s">
+        <v>127</v>
+      </c>
       <c r="K101" s="47">
         <v>95</v>
       </c>
       <c r="L101" s="45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M101" s="51" t="str">
         <f>I21</f>
@@ -3171,15 +3531,18 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="11:18">
+    <row r="102" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J102" t="s">
+        <v>106</v>
+      </c>
       <c r="K102" s="47">
         <v>96</v>
       </c>
       <c r="L102" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M102" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -3191,12 +3554,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="103" spans="11:18">
+    <row r="103" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J103" t="s">
+        <v>106</v>
+      </c>
       <c r="K103" s="2">
         <v>97</v>
       </c>
       <c r="L103" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
@@ -3207,12 +3573,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="11:18">
+    <row r="104" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>108</v>
+      </c>
       <c r="K104" s="47">
         <v>98</v>
       </c>
       <c r="L104" s="33" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="M104" s="33" t="str">
         <f>I19</f>
@@ -3228,12 +3597,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="105" spans="11:18">
+    <row r="105" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K105" s="2">
         <v>99</v>
       </c>
       <c r="L105" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -3244,12 +3613,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="106" spans="11:18">
+    <row r="106" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K106" s="2">
         <v>100</v>
       </c>
       <c r="L106" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
@@ -3260,7 +3629,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="121" spans="16:16">
+    <row r="121" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P121" t="s">
         <v>0</v>
       </c>
@@ -3405,12 +3774,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3419,14 +3782,43 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E1E2B25-4F68-476B-9D06-ECE7D7777F55}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E1E2B25-4F68-476B-9D06-ECE7D7777F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="928a6cc6-ffac-4375-bcba-2877d4e01fda"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D65A50C6-7452-4F91-A606-C672C412412F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B01474-8399-42A1-95B1-D32610A94D18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B01474-8399-42A1-95B1-D32610A94D18}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D65A50C6-7452-4F91-A606-C672C412412F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
alle deteien hinzugefügt oder erneuert
</commit_message>
<xml_diff>
--- a/files/Fragen.xlsx
+++ b/files/Fragen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20339"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sp01\mldata\benutzer\sus\golze.paul\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C7A3DB-E3BB-451D-A8FF-431184D5AC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1834B9-9EC7-4DA8-ABD7-E2BCED51A96F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FEFB16A5-D4A0-4625-B94E-FC4230FEBFEF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{FEFB16A5-D4A0-4625-B94E-FC4230FEBFEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -43,10 +32,19 @@
   <commentList>
     <comment ref="T93" authorId="0" shapeId="0" xr:uid="{FD4F012B-4165-4CA4-8719-6EF93C4E1C66}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     ok</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -54,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="142">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -481,6 +479,21 @@
   </si>
   <si>
     <t>Was genau hast du um 15:45 Uhr gemacht?</t>
+  </si>
+  <si>
+    <t>Ich weiß es nicht</t>
+  </si>
+  <si>
+    <t>Ich möchte dazu keine Auskunft geben</t>
+  </si>
+  <si>
+    <t>Ich war hauptsächlich zu Hause, frag meine Freundin</t>
+  </si>
+  <si>
+    <t>Ich war nur zu Hause, ich habe geschlafen und gegessen</t>
+  </si>
+  <si>
+    <t>Antworten:</t>
   </si>
 </sst>
 </file>
@@ -1236,15 +1249,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FE7B2B-B244-4DB1-96E1-1BBBEAD0F830}">
   <dimension ref="E1:T121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="J85" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="61" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.5703125" bestFit="1" customWidth="1"/>
@@ -1409,6 +1422,9 @@
       <c r="I11" s="15" t="s">
         <v>18</v>
       </c>
+      <c r="J11" t="s">
+        <v>137</v>
+      </c>
       <c r="K11" s="47">
         <v>5</v>
       </c>
@@ -2082,6 +2098,13 @@
       </c>
     </row>
     <row r="36" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>141</v>
+      </c>
+      <c r="I36" s="53">
+        <f>COUNTA(J7:J106)</f>
+        <v>100</v>
+      </c>
       <c r="J36" t="s">
         <v>125</v>
       </c>
@@ -2392,6 +2415,9 @@
       </c>
     </row>
     <row r="50" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>138</v>
+      </c>
       <c r="K50" s="47">
         <v>44</v>
       </c>
@@ -2495,6 +2521,9 @@
       </c>
     </row>
     <row r="55" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>139</v>
+      </c>
       <c r="K55" s="47">
         <v>49</v>
       </c>
@@ -2561,6 +2590,9 @@
       </c>
     </row>
     <row r="58" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>137</v>
+      </c>
       <c r="K58" s="2">
         <v>52</v>
       </c>
@@ -3116,6 +3148,9 @@
       </c>
     </row>
     <row r="83" spans="10:20" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>140</v>
+      </c>
       <c r="K83" s="47">
         <v>77</v>
       </c>
@@ -3598,6 +3633,9 @@
       </c>
     </row>
     <row r="105" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J105" t="s">
+        <v>140</v>
+      </c>
       <c r="K105" s="2">
         <v>99</v>
       </c>
@@ -3614,6 +3652,9 @@
       </c>
     </row>
     <row r="106" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>138</v>
+      </c>
       <c r="K106" s="2">
         <v>100</v>
       </c>
@@ -3642,6 +3683,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010058973979E6C2944FA226012469FF5F8D" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="e6cb80843580629beb26c4934525366c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="928a6cc6-ffac-4375-bcba-2877d4e01fda" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a12ff516b0fb2ba8d62f671bc3e9ba8" ns3:_="">
     <xsd:import namespace="928a6cc6-ffac-4375-bcba-2877d4e01fda"/>
@@ -3773,22 +3829,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D65A50C6-7452-4F91-A606-C672C412412F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B01474-8399-42A1-95B1-D32610A94D18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E1E2B25-4F68-476B-9D06-ECE7D7777F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3804,21 +3862,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B01474-8399-42A1-95B1-D32610A94D18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D65A50C6-7452-4F91-A606-C672C412412F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>